<commit_message>
Add name-by-name comparison mode, add logging
- add new comparison mode ("name-by-name"), which is invoked by
  appending the flag "--by-name"
- add logging: write debug info to a file
- remove code redundancy, minor improvements
</commit_message>
<xml_diff>
--- a/tests/data/test_PS-table_modified.xlsx
+++ b/tests/data/test_PS-table_modified.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -34,10 +34,16 @@
     <t xml:space="preserve">L1_SingleMuCosmics</t>
   </si>
   <si>
+    <t xml:space="preserve">L1_DoubleMu0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1_DoubleMu0_SQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1_SingleMu28</t>
+  </si>
+  <si>
     <t xml:space="preserve">L1_SingleMuOpen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L1_SingleMu28</t>
   </si>
 </sst>
 </file>
@@ -150,12 +156,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -248,12 +254,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,76 +343,148 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="J3" s="4" t="n">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="K3" s="4" t="n">
-        <v>8</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>500</v>
+        <v>110</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="D4" s="4" t="n">
+        <v>111</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>112</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>113</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>114</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>115</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>116</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E5" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F5" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G5" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H5" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I5" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J5" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K5" s="4" t="n">
         <v>30</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:K3">
+  <conditionalFormatting sqref="C2:K6">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>1</formula>
     </cfRule>
@@ -414,105 +492,6 @@
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" priority="5" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" priority="8" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" priority="11" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" priority="14" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" priority="17" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" priority="20" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" priority="23" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" priority="26" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" priority="29" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>